<commit_message>
Corrected error in currency conversion factor.
</commit_message>
<xml_diff>
--- a/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
+++ b/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\World Resources Institute\TRAC City - HK 2050 is now\EPS HK 2.0\eps-hongkong-web\InputData\web-app\OCCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-hongkong\InputData\web-app\OCCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_83805BC7E8E24D732DCF0CC861954D85F9C6248B" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9301B022-3D3C-4C18-946F-9CB2B8B1E35A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="OCCF-DpMOCU" sheetId="4" r:id="rId3"/>
     <sheet name="OCCF-DpSOCU" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -122,16 +121,16 @@
     <t>Recall, this variable is "dollars per large/medium/small currency output unit"</t>
   </si>
   <si>
-    <t>USD converted to HKD</t>
-  </si>
-  <si>
     <t>this number was used</t>
   </si>
+  <si>
+    <t>HKD converted to USD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -279,23 +278,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -331,23 +313,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -523,11 +488,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,19 +636,19 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>7.8285</v>
+        <v>0.12773839177364757</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>A26*A35</f>
-        <v>7.1578117256786946</v>
+        <v>0.11679470632391308</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -693,13 +658,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -719,7 +684,7 @@
       </c>
       <c r="B2" s="7">
         <f>10^9*About!$A$36</f>
-        <v>7157811725.6786947</v>
+        <v>116794706.32391308</v>
       </c>
     </row>
   </sheetData>
@@ -728,7 +693,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -754,7 +719,7 @@
       </c>
       <c r="B2" s="7">
         <f>10^6*About!$A$36</f>
-        <v>7157811.7256786944</v>
+        <v>116794.70632391308</v>
       </c>
     </row>
   </sheetData>
@@ -763,7 +728,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -789,7 +754,7 @@
       </c>
       <c r="B2" s="6">
         <f>1*About!A36</f>
-        <v>7.1578117256786946</v>
+        <v>0.11679470632391308</v>
       </c>
     </row>
   </sheetData>
@@ -798,21 +763,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1050,19 +1015,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D1E47CE-7FF8-41C0-9A62-3DDD9BF31744}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8916BED6-C418-4D2C-92B1-9B25D4D2165C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D1E47CE-7FF8-41C0-9A62-3DDD9BF31744}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>